<commit_message>
Adding inverter to BOM
Inverter was missing from BOM, correctec
</commit_message>
<xml_diff>
--- a/StarlinkFrontRunnerBOM.xlsx
+++ b/StarlinkFrontRunnerBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robkikta/Development/StarRunner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75748798-DCF5-0846-A611-904AAF049BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4E0851-5BA4-974E-8384-93EACABC70F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="6780" windowWidth="36680" windowHeight="20160" xr2:uid="{AD64AF22-FFE9-7744-B65D-54CC2456CAEB}"/>
+    <workbookView xWindow="1280" yWindow="6780" windowWidth="36680" windowHeight="20160" xr2:uid="{AD64AF22-FFE9-7744-B65D-54CC2456CAEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>Part Name</t>
   </si>
@@ -261,6 +261,21 @@
   </si>
   <si>
     <t>Updated: 21-Jan-2023</t>
+  </si>
+  <si>
+    <t>Inverter</t>
+  </si>
+  <si>
+    <t>Victron</t>
+  </si>
+  <si>
+    <t>Phoenix 250VA 12-Volt 120V AC Pure Sine Wave Inverter</t>
+  </si>
+  <si>
+    <t>Phoenix 250VA</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B01NAO10QX/ref=ox_sc_act_image_1?smid=AERMGYAT5R869&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -916,10 +931,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I20"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" ref="H5:H18" si="0">F5*G5</f>
+        <f t="shared" ref="H5:H19" si="0">F5*G5</f>
         <v>69</v>
       </c>
       <c r="I5" s="10" t="s">
@@ -1081,7 +1096,9 @@
       <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
@@ -1128,266 +1145,293 @@
     </row>
     <row r="10" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="F10" s="9">
-        <v>7.69</v>
+        <v>96.9</v>
       </c>
       <c r="G10" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>15.38</v>
+        <v>96.9</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F11" s="9">
-        <v>30</v>
+        <v>7.69</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
+        <v>15.38</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="9">
         <v>30</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="9">
-        <v>18.11</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>18.11</v>
+        <v>30</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9">
-        <v>5.5</v>
+        <v>18.11</v>
       </c>
       <c r="G13" s="6">
         <v>1</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>18.11</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F14" s="9">
-        <v>22.46</v>
+        <v>5.5</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>22.46</v>
+        <v>5.5</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="F15" s="9">
-        <v>4.97</v>
+        <v>22.46</v>
       </c>
       <c r="G15" s="6">
         <v>1</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
+        <v>22.46</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="9">
         <v>4.97</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="9">
-        <v>5.38</v>
       </c>
       <c r="G16" s="6">
         <v>1</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="0"/>
-        <v>5.38</v>
+        <v>4.97</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F17" s="9">
-        <v>0.66</v>
+        <v>5.38</v>
       </c>
       <c r="G17" s="6">
         <v>1</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="0"/>
+        <v>5.38</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="9">
         <v>0.66</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+    <row r="19" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C19" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E19" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F19" s="26">
         <v>43.8</v>
       </c>
-      <c r="G18" s="23">
-        <v>1</v>
-      </c>
-      <c r="H18" s="26">
+      <c r="G19" s="23">
+        <v>1</v>
+      </c>
+      <c r="H19" s="26">
         <f t="shared" si="0"/>
         <v>43.8</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I19" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
+    <row r="20" spans="2:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="28">
-        <f>SUM(H4:H18)</f>
-        <v>758.45</v>
-      </c>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="20" spans="2:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="28">
+        <f>SUM(H4:H19)</f>
+        <v>855.35</v>
+      </c>
+      <c r="I20" s="29"/>
+    </row>
+    <row r="21" spans="2:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{41E33B09-60DA-C547-9CDC-045955355519}"/>
@@ -1396,13 +1440,14 @@
     <hyperlink ref="I7" r:id="rId4" xr:uid="{A5850616-C37D-ED45-84F9-0305DA8E35D4}"/>
     <hyperlink ref="I6" r:id="rId5" xr:uid="{7AB8D469-5DEE-6043-9AA0-B43A8933F0B0}"/>
     <hyperlink ref="I5" r:id="rId6" xr:uid="{8709F4FA-7286-2B43-8D16-DF11F77693E6}"/>
-    <hyperlink ref="I10" r:id="rId7" xr:uid="{0E8E08B4-A782-954C-A1A1-1CC5663EDB31}"/>
-    <hyperlink ref="I16" r:id="rId8" xr:uid="{8415CDCE-5793-CB40-981B-32667FF96C2B}"/>
-    <hyperlink ref="I17" r:id="rId9" xr:uid="{ECCF0CF1-4369-3646-A696-4A91DB97AEBD}"/>
-    <hyperlink ref="I18" r:id="rId10" xr:uid="{5C566A00-6CB9-B647-8705-62BBF6C5729F}"/>
-    <hyperlink ref="I12" r:id="rId11" xr:uid="{9259C151-1E33-5B4F-9020-3EB2D2FD294D}"/>
-    <hyperlink ref="I14" r:id="rId12" xr:uid="{D341FB9A-89AC-8749-A661-4552D5201D64}"/>
-    <hyperlink ref="I13" r:id="rId13" xr:uid="{AAD471BD-BC18-284C-8A09-6B8F7DFBDE60}"/>
+    <hyperlink ref="I11" r:id="rId7" xr:uid="{0E8E08B4-A782-954C-A1A1-1CC5663EDB31}"/>
+    <hyperlink ref="I17" r:id="rId8" xr:uid="{8415CDCE-5793-CB40-981B-32667FF96C2B}"/>
+    <hyperlink ref="I18" r:id="rId9" xr:uid="{ECCF0CF1-4369-3646-A696-4A91DB97AEBD}"/>
+    <hyperlink ref="I19" r:id="rId10" xr:uid="{5C566A00-6CB9-B647-8705-62BBF6C5729F}"/>
+    <hyperlink ref="I13" r:id="rId11" xr:uid="{9259C151-1E33-5B4F-9020-3EB2D2FD294D}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{D341FB9A-89AC-8749-A661-4552D5201D64}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{AAD471BD-BC18-284C-8A09-6B8F7DFBDE60}"/>
+    <hyperlink ref="I10" r:id="rId14" xr:uid="{B29712FB-3FAD-0944-BA12-28B59F4093C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="56" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>